<commit_message>
8ka i 1 fixed
</commit_message>
<xml_diff>
--- a/1/1.xlsx
+++ b/1/1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mskrz\Desktop\Github\Fizyka-laby\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pulpit\Github\Fizyka-laby\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15556C0-C70F-4F8D-94E5-A1FAA34B5C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9F4572-6197-42D2-8398-E0292D259BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1875" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pomiary" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,6 +253,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -290,6 +290,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Zadanie 5. Zależność </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>T(L)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -315,7 +344,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -361,6 +390,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -562,9 +606,434 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1290262768"/>
+        <c:axId val="1290263248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1290262768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.55000000000000004"/>
+          <c:min val="0.15000000000000002"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>L, m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1290263248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1290263248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T, s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1290262768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Zadanie 6. Zależność</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>√L, √m </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6163648554653749E-2"/>
+          <c:y val="0.10308309865030968"/>
+          <c:w val="0.75108994802326023"/>
+          <c:h val="0.82493062236617087"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:v>T(√L)</c:v>
           </c:tx>
@@ -800,7 +1269,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1F6C-45B4-B6EA-23B5FF3F498D}"/>
+              <c16:uniqueId val="{00000002-A98A-401E-85C5-6745A545D84A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -819,8 +1288,8 @@
         <c:axId val="1290262768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.8"/>
-          <c:min val="0.1"/>
+          <c:max val="0.75000000000000011"/>
+          <c:min val="0.35000000000000003"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -839,6 +1308,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>√L, √m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -864,7 +1358,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -902,7 +1396,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1290263248"/>
@@ -933,6 +1427,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T, s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -958,7 +1477,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pl-PL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -996,7 +1515,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1290262768"/>
@@ -1038,7 +1557,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1075,7 +1594,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pl-PL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1126,6 +1645,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1642,20 +2201,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:colOff>232262</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>98423</xdr:rowOff>
+      <xdr:rowOff>183903</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>187243</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>280866</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>77338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1675,6 +2750,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>183173</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>36635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>354134</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>125455</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB8E703-DDF8-4471-8556-467010B22C3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1952,27 +3065,27 @@
       <selection activeCell="C3" sqref="C3:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.1796875" style="1"/>
-    <col min="4" max="8" width="6.7265625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <f>2.2/2</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1998,7 +3111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2027,7 +3140,7 @@
         <v>14.28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -2056,7 +3169,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -2085,7 +3198,7 @@
         <v>12.67</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -2114,7 +3227,7 @@
         <v>11.86</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -2143,7 +3256,7 @@
         <v>11.17</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -2172,7 +3285,7 @@
         <v>10.029999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -2201,7 +3314,7 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -2230,16 +3343,16 @@
         <v>7.77</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D13" s="3" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2277,7 +3390,7 @@
         <v>14.12</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -2315,7 +3428,7 @@
         <v>13.46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -2353,7 +3466,7 @@
         <v>12.71</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -2391,7 +3504,7 @@
         <v>11.87</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -2429,7 +3542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>5</v>
       </c>
@@ -2467,7 +3580,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -2505,7 +3618,7 @@
         <v>8.91</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>7</v>
       </c>
@@ -2543,7 +3656,7 @@
         <v>7.72</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>8</v>
       </c>
@@ -2579,30 +3692,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE558D6-0013-4279-ABD3-653D2E89192F}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="78" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26:Q27"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
-    <col min="2" max="2" width="5.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="6.1796875" style="1" customWidth="1"/>
-    <col min="10" max="12" width="5.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.36328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="1"/>
+    <col min="5" max="9" width="6.140625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="5.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
     <col min="15" max="17" width="7" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1796875" style="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>0.004/SQRT(3)</f>
         <v>2.3094010767585032E-3</v>
@@ -2610,14 +3723,14 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="str">
+      <c r="E2" s="6" t="str">
         <f>Pomiary!D1</f>
         <v>t, s</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
@@ -2625,7 +3738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2685,7 +3798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.141</v>
       </c>
@@ -2693,11 +3806,11 @@
         <f>Pomiary!B3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <f>Pomiary!C3</f>
         <v>0.501</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f>SQRT(C4)</f>
         <v>0.70781353476745557</v>
       </c>
@@ -2754,7 +3867,7 @@
         <v>1,4114(58)</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2762,11 +3875,11 @@
         <f>Pomiary!B4</f>
         <v>2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f>Pomiary!C4</f>
         <v>0.45100000000000001</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" ref="D5:D11" si="0">SQRT(C5)</f>
         <v>0.67156533561523257</v>
       </c>
@@ -2823,7 +3936,7 @@
         <v>1,3458(58)</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>0.1/SQRT(3)</f>
         <v>5.7735026918962581E-2</v>
@@ -2832,11 +3945,11 @@
         <f>Pomiary!B5</f>
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f>Pomiary!C5</f>
         <v>0.40100000000000002</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>0.63324560795950258</v>
       </c>
@@ -2893,7 +4006,7 @@
         <v>1,2706(57)</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2901,11 +4014,11 @@
         <f>Pomiary!B6</f>
         <v>4</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>Pomiary!C6</f>
         <v>0.35100000000000003</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>0.59245252974394502</v>
       </c>
@@ -2962,7 +4075,7 @@
         <v>1,1860(57)</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10</v>
       </c>
@@ -2970,11 +4083,11 @@
         <f>Pomiary!B7</f>
         <v>5</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f>Pomiary!C7</f>
         <v>0.311</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>0.55767373974394741</v>
       </c>
@@ -3031,16 +4144,16 @@
         <v>1,1010(57)</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f>Pomiary!B8</f>
         <v>6</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f>Pomiary!C8</f>
         <v>0.251</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>0.5009990019950139</v>
       </c>
@@ -3097,16 +4210,16 @@
         <v>0,9986(58)</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f>Pomiary!B9</f>
         <v>7</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f>Pomiary!C9</f>
         <v>0.20100000000000001</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>0.44833023542919792</v>
       </c>
@@ -3163,16 +4276,16 @@
         <v>0,8908(58)</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f>Pomiary!B10</f>
         <v>8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f>Pomiary!C10</f>
         <v>0.151</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>0.38858718455450897</v>
       </c>
@@ -3229,17 +4342,17 @@
         <v>0,7720(58)</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3247,7 +4360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q16" s="2">
         <f t="array" ref="Q16:R18">LINEST(O4:O11,D4:D11,TRUE,TRUE)</f>
         <v>2.0215077668947425</v>
@@ -3256,7 +4369,7 @@
         <v>-1.5241704997084327E-2</v>
       </c>
     </row>
-    <row r="17" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3270,7 +4383,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P18" s="2" t="s">
         <v>23</v>
       </c>
@@ -3281,7 +4394,7 @@
         <v>5.8143705495192922E-3</v>
       </c>
     </row>
-    <row r="21" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P21" s="1" t="s">
         <v>24</v>
       </c>
@@ -3289,7 +4402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P22" s="1" t="s">
         <v>25</v>
       </c>
@@ -3300,8 +4413,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="16:19" x14ac:dyDescent="0.35">
-      <c r="P23" s="4">
+    <row r="23" spans="16:19" x14ac:dyDescent="0.25">
+      <c r="P23" s="3">
         <f>4*PI()*PI()/Q16/Q16</f>
         <v>9.66070694585515</v>
       </c>
@@ -3314,12 +4427,12 @@
         <v>9,66(18)</v>
       </c>
     </row>
-    <row r="25" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P26" s="2" t="s">
         <v>29</v>
       </c>
@@ -3327,7 +4440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="16:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:19" x14ac:dyDescent="0.25">
       <c r="P27" s="2">
         <f>ABS(P23-9.8)</f>
         <v>0.13929305414485071</v>
@@ -3354,16 +4467,16 @@
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -3380,14 +4493,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>0.501</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.70781353476745557</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>6.5047008001907995E-3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3397,14 +4510,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>0.45100000000000001</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.67156533561523257</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>6.2495143811342286E-3</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -3414,14 +4527,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>0.40100000000000002</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.63324560795950258</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>5.1027071246548652E-3</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -3431,14 +4544,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>0.35100000000000003</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.59245252974394502</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>4.0340441866691676E-3</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -3448,14 +4561,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>0.311</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.55767373974394741</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>4.0340441866691676E-3</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -3465,14 +4578,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>0.251</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>0.5009990019950139</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>6.5047008001904438E-3</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -3482,14 +4595,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>0.20100000000000001</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>0.44833023542919792</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>6.2495143811338123E-3</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3499,14 +4612,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>0.151</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>0.38858718455450897</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>6.9871694912890733E-3</v>
       </c>
       <c r="D9" s="2" t="s">

</xml_diff>